<commit_message>
construidos dataframes con tasa positiva
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -2283,7 +2283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E2:F323"/>
+  <dimension ref="E2:F324"/>
   <sheetViews>
     <sheetView topLeftCell="A269" workbookViewId="0">
       <selection activeCell="F254" sqref="F254:F303"/>
@@ -5514,6 +5514,16 @@
         <v>7.3</v>
       </c>
     </row>
+    <row r="324">
+      <c r="E324" t="inlineStr">
+        <is>
+          <t>30-11-2022</t>
+        </is>
+      </c>
+      <c r="F324" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ahora va todo automático, incluso generar el chart de BTC y grabarlo
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -2283,7 +2283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E2:F324"/>
+  <dimension ref="E2:F328"/>
   <sheetViews>
     <sheetView topLeftCell="A269" workbookViewId="0">
       <selection activeCell="F254" sqref="F254:F303"/>
@@ -5524,6 +5524,46 @@
         <v>7.3</v>
       </c>
     </row>
+    <row r="325">
+      <c r="E325" t="inlineStr">
+        <is>
+          <t>01-12-2022</t>
+        </is>
+      </c>
+      <c r="F325" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="E326" t="inlineStr">
+        <is>
+          <t>02-12-2022</t>
+        </is>
+      </c>
+      <c r="F326" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="327">
+      <c r="E327" t="inlineStr">
+        <is>
+          <t>03-12-2022</t>
+        </is>
+      </c>
+      <c r="F327" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="E328" t="inlineStr">
+        <is>
+          <t>04-12-2022</t>
+        </is>
+      </c>
+      <c r="F328" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding support for USD charts and hiding twitter keys
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -2283,7 +2283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E2:F328"/>
+  <dimension ref="E2:F329"/>
   <sheetViews>
     <sheetView topLeftCell="A269" workbookViewId="0">
       <selection activeCell="F254" sqref="F254:F303"/>
@@ -5564,6 +5564,16 @@
         <v>7.3</v>
       </c>
     </row>
+    <row r="329">
+      <c r="E329" t="inlineStr">
+        <is>
+          <t>05-12-2022</t>
+        </is>
+      </c>
+      <c r="F329" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
it now tweets both BTC and USD charts
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -2283,7 +2283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E2:F329"/>
+  <dimension ref="E2:F330"/>
   <sheetViews>
     <sheetView topLeftCell="A269" workbookViewId="0">
       <selection activeCell="F254" sqref="F254:F303"/>
@@ -5574,6 +5574,16 @@
         <v>7.3</v>
       </c>
     </row>
+    <row r="330">
+      <c r="E330" t="inlineStr">
+        <is>
+          <t>06-12-2022</t>
+        </is>
+      </c>
+      <c r="F330" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the bitcoin_price growth rate parameter and it looks now better
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -2283,7 +2283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E2:F330"/>
+  <dimension ref="E2:F333"/>
   <sheetViews>
     <sheetView topLeftCell="A269" workbookViewId="0">
       <selection activeCell="F254" sqref="F254:F303"/>
@@ -5584,6 +5584,36 @@
         <v>7.3</v>
       </c>
     </row>
+    <row r="331">
+      <c r="E331" t="inlineStr">
+        <is>
+          <t>07-12-2022</t>
+        </is>
+      </c>
+      <c r="F331" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="E332" t="inlineStr">
+        <is>
+          <t>08-12-2022</t>
+        </is>
+      </c>
+      <c r="F332" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="E333" t="inlineStr">
+        <is>
+          <t>09-12-2022</t>
+        </is>
+      </c>
+      <c r="F333" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
awesome profitability table generation
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -2283,7 +2283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E2:F333"/>
+  <dimension ref="E2:F335"/>
   <sheetViews>
     <sheetView topLeftCell="A269" workbookViewId="0">
       <selection activeCell="F254" sqref="F254:F303"/>
@@ -5614,6 +5614,26 @@
         <v>7.3</v>
       </c>
     </row>
+    <row r="334">
+      <c r="E334" t="inlineStr">
+        <is>
+          <t>10-12-2022</t>
+        </is>
+      </c>
+      <c r="F334" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="335">
+      <c r="E335" t="inlineStr">
+        <is>
+          <t>11-12-2022</t>
+        </is>
+      </c>
+      <c r="F335" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
adding the ability to create charts for custom requests
</commit_message>
<xml_diff>
--- a/pruebas.xlsx
+++ b/pruebas.xlsx
@@ -2283,7 +2283,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="E2:F335"/>
+  <dimension ref="E2:F338"/>
   <sheetViews>
     <sheetView topLeftCell="A269" workbookViewId="0">
       <selection activeCell="F254" sqref="F254:F303"/>
@@ -5634,6 +5634,36 @@
         <v>7.3</v>
       </c>
     </row>
+    <row r="336">
+      <c r="E336" t="inlineStr">
+        <is>
+          <t>12-12-2022</t>
+        </is>
+      </c>
+      <c r="F336" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="337">
+      <c r="E337" t="inlineStr">
+        <is>
+          <t>13-12-2022</t>
+        </is>
+      </c>
+      <c r="F337" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="338">
+      <c r="E338" t="inlineStr">
+        <is>
+          <t>14-12-2022</t>
+        </is>
+      </c>
+      <c r="F338" t="n">
+        <v>7.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>